<commit_message>
Atualização automática de CAMAQUA.xlsx
</commit_message>
<xml_diff>
--- a/CAMAQUA.xlsx
+++ b/CAMAQUA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A256D564-ABA2-4AE4-80B4-5978E20CA137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A0B2D3AD-6662-4DE5-BA6A-2DC658E69BAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,20 +22,7 @@
     <sheet name="Recolhimento x Eliminacao" sheetId="6" r:id="rId7"/>
     <sheet name="Desarquivamentos Pendentes" sheetId="7" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -1148,7 +1135,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1208,36 +1195,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1276,14 +1239,9 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1336,7 +1294,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{0081834B-83BA-4065-9116-AF2729FC86FD}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{18EBC92F-C497-464D-A293-929D7927D169}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1366,10 +1324,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{351FD6CE-8E02-4CDD-8B5E-2A127D86A05F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D5426D2-8080-45BD-A8BF-0071EDC0AC8C}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1407,7 +1365,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BEB7F7E-467D-4A59-B575-E87F4DDED651}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F4BB490-D96B-4E32-8457-02E779B3C439}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1470,7 +1428,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E4092AD-E41A-49DF-A0AF-266D354F9E64}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{765A8FD4-5339-468A-805E-8F52D6429013}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1489,7 +1447,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B580FECD-3709-BBEC-753E-123367D3E6EC}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B267E2B4-4F47-4DAC-4156-DC12C4DCFEDB}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1538,7 +1496,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99663490-A37A-4BFA-EC47-8B844A635288}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F87B189B-5AC9-FB42-6BCF-2BD2309A60B9}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1557,7 +1515,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BEE62C8-B8BD-F810-6E18-D264BBEEF3F5}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A0420E2-2CAE-3756-6C5F-51B1426D7BFC}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1588,7 +1546,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25CC9A19-BDBC-709E-337A-078F9D5B1FD8}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{220C399C-4327-46F2-D639-AD66F261C230}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1619,7 +1577,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08C47CD0-7B07-73E6-2281-4BF0F15C958D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{739DFB78-D122-C9BD-CC2E-B7A356F75C44}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1662,7 +1620,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D58A41D-344E-4699-9C9F-3F1C6D06FCF0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56329E1C-366E-42BE-B560-0FF7DF2787DB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1700,7 +1658,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58F2878D-F22F-4D88-B19D-6E3420E8A1BC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{153B0EB2-92F8-4E41-8C2F-AF34B43835BC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1743,7 +1701,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2AF13CFE-7DDD-4B13-8BDD-DC608CE47CAE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA256562-08DC-4B70-A062-5425F0F97245}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2056,7 +2014,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCB352D8-3916-46DC-8225-E5B87C91C440}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A476907-E942-43D4-8597-D68D3E8146B0}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -2068,98 +2026,98 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="12.5703125" style="40"/>
-    <col min="6" max="6" width="2" style="40" customWidth="1"/>
-    <col min="7" max="16" width="13.42578125" style="40" customWidth="1"/>
-    <col min="17" max="16384" width="12.5703125" style="40"/>
+    <col min="1" max="5" width="12.5703125" style="37"/>
+    <col min="6" max="6" width="2" style="37" customWidth="1"/>
+    <col min="7" max="16" width="13.42578125" style="37" customWidth="1"/>
+    <col min="17" max="16384" width="12.5703125" style="37"/>
   </cols>
   <sheetData>
     <row r="1" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F1" s="39"/>
+      <c r="F1" s="36"/>
     </row>
     <row r="2" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F2" s="39"/>
+      <c r="F2" s="36"/>
     </row>
     <row r="3" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F3" s="39"/>
+      <c r="F3" s="36"/>
     </row>
     <row r="4" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F4" s="39"/>
+      <c r="F4" s="36"/>
     </row>
     <row r="5" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F5" s="39"/>
+      <c r="F5" s="36"/>
     </row>
     <row r="6" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F6" s="39"/>
+      <c r="F6" s="36"/>
     </row>
     <row r="7" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F7" s="39"/>
+      <c r="F7" s="36"/>
     </row>
     <row r="8" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F8" s="39"/>
+      <c r="F8" s="36"/>
     </row>
     <row r="9" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F9" s="39"/>
+      <c r="F9" s="36"/>
     </row>
     <row r="10" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F10" s="39"/>
+      <c r="F10" s="36"/>
     </row>
     <row r="11" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F11" s="39"/>
+      <c r="F11" s="36"/>
     </row>
     <row r="12" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F12" s="39"/>
+      <c r="F12" s="36"/>
     </row>
     <row r="13" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F13" s="39"/>
+      <c r="F13" s="36"/>
     </row>
     <row r="14" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F14" s="39"/>
+      <c r="F14" s="36"/>
     </row>
     <row r="15" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F15" s="39"/>
+      <c r="F15" s="36"/>
     </row>
     <row r="16" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F16" s="39"/>
+      <c r="F16" s="36"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F17" s="39"/>
+      <c r="F17" s="36"/>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F18" s="39"/>
+      <c r="F18" s="36"/>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F19" s="39"/>
+      <c r="F19" s="36"/>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F20" s="39"/>
+      <c r="F20" s="36"/>
     </row>
     <row r="21" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F21" s="39"/>
+      <c r="F21" s="36"/>
     </row>
     <row r="22" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F22" s="39"/>
+      <c r="F22" s="36"/>
     </row>
     <row r="23" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F23" s="39"/>
+      <c r="F23" s="36"/>
     </row>
     <row r="24" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F24" s="39"/>
+      <c r="F24" s="36"/>
     </row>
     <row r="25" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F25" s="39"/>
+      <c r="F25" s="36"/>
     </row>
     <row r="26" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F26" s="39"/>
+      <c r="F26" s="36"/>
     </row>
     <row r="27" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F27" s="39"/>
+      <c r="F27" s="36"/>
     </row>
     <row r="28" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F28" s="39"/>
+      <c r="F28" s="36"/>
     </row>
     <row r="29" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F29" s="39"/>
+      <c r="F29" s="36"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5451,19 +5409,19 @@
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="2" t="s">
         <v>276</v>
       </c>
     </row>
@@ -5486,46 +5444,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="18" t="s">
         <v>277</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="17" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="19" t="s">
         <v>279</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="19" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="19" t="s">
         <v>281</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="19" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="19" t="s">
         <v>283</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="19" t="s">
         <v>282</v>
       </c>
     </row>
@@ -5543,16 +5501,16 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
     <col min="3" max="3" width="37.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="20" customWidth="1"/>
-    <col min="8" max="8" width="43.42578125" customWidth="1"/>
-    <col min="9" max="9" width="27.85546875" customWidth="1"/>
-    <col min="10" max="10" width="39.7109375" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" customWidth="1"/>
+    <col min="8" max="8" width="47.5703125" customWidth="1"/>
+    <col min="9" max="9" width="89" customWidth="1"/>
+    <col min="10" max="10" width="72.85546875" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5586,7 +5544,7 @@
       <c r="J1" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="K1" s="20" t="s">
         <v>293</v>
       </c>
     </row>
@@ -5600,10 +5558,10 @@
       <c r="C2" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="D2" s="24">
+      <c r="D2" s="21">
         <v>614.25</v>
       </c>
-      <c r="E2" s="24">
+      <c r="E2" s="21">
         <v>61.43</v>
       </c>
       <c r="F2" s="2">
@@ -5621,7 +5579,7 @@
       <c r="J2" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="K2" s="25">
+      <c r="K2" s="22">
         <v>11019</v>
       </c>
     </row>
@@ -5635,10 +5593,10 @@
       <c r="C3" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="D3" s="24">
+      <c r="D3" s="21">
         <v>17885.689999999999</v>
       </c>
-      <c r="E3" s="24">
+      <c r="E3" s="21">
         <v>1788.57</v>
       </c>
       <c r="F3" s="2">
@@ -5656,7 +5614,7 @@
       <c r="J3" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K3" s="25">
+      <c r="K3" s="22">
         <v>12520</v>
       </c>
     </row>
@@ -5670,10 +5628,10 @@
       <c r="C4" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="D4" s="24">
+      <c r="D4" s="21">
         <v>2627</v>
       </c>
-      <c r="E4" s="24">
+      <c r="E4" s="21">
         <v>262.7</v>
       </c>
       <c r="F4" s="2">
@@ -5691,7 +5649,7 @@
       <c r="J4" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="K4" s="25">
+      <c r="K4" s="22">
         <v>29328</v>
       </c>
     </row>
@@ -5705,10 +5663,10 @@
       <c r="C5" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="21">
         <v>600</v>
       </c>
-      <c r="E5" s="24">
+      <c r="E5" s="21">
         <v>60</v>
       </c>
       <c r="F5" s="2">
@@ -5726,7 +5684,7 @@
       <c r="J5" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="K5" s="25">
+      <c r="K5" s="22">
         <v>29328</v>
       </c>
     </row>
@@ -5751,54 +5709,55 @@
     <col min="6" max="6" width="12.5703125" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="14" width="13" customWidth="1"/>
-    <col min="15" max="15" width="30.85546875" customWidth="1"/>
+    <col min="9" max="12" width="13" customWidth="1"/>
+    <col min="13" max="13" width="42.140625" customWidth="1"/>
+    <col min="14" max="15" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="23" t="s">
         <v>305</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="24" t="s">
         <v>306</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="24" t="s">
         <v>307</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="24" t="s">
         <v>308</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="24" t="s">
         <v>309</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="F1" s="25" t="s">
         <v>310</v>
       </c>
-      <c r="G1" s="28" t="s">
+      <c r="G1" s="25" t="s">
         <v>311</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="23" t="s">
         <v>312</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="I1" s="23" t="s">
         <v>313</v>
       </c>
-      <c r="J1" s="26" t="s">
+      <c r="J1" s="23" t="s">
         <v>314</v>
       </c>
-      <c r="K1" s="26" t="s">
+      <c r="K1" s="23" t="s">
         <v>315</v>
       </c>
-      <c r="L1" s="26" t="s">
+      <c r="L1" s="23" t="s">
         <v>316</v>
       </c>
-      <c r="M1" s="26" t="s">
+      <c r="M1" s="23" t="s">
         <v>317</v>
       </c>
-      <c r="N1" s="26" t="s">
+      <c r="N1" s="23" t="s">
         <v>318</v>
       </c>
-      <c r="O1" s="26" t="s">
+      <c r="O1" s="23" t="s">
         <v>319</v>
       </c>
     </row>
@@ -5809,41 +5768,41 @@
       <c r="B2" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="C2" s="29">
+      <c r="C2" s="26">
         <v>45717</v>
       </c>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30" t="s">
+      <c r="D2" s="27"/>
+      <c r="E2" s="27" t="s">
         <v>321</v>
       </c>
-      <c r="F2" s="31">
+      <c r="F2" s="28">
         <v>15752</v>
       </c>
-      <c r="G2" s="31">
+      <c r="G2" s="28">
         <v>2365</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="I2" s="32" t="s">
+      <c r="I2" s="29" t="s">
         <v>323</v>
       </c>
-      <c r="J2" s="32" t="s">
+      <c r="J2" s="29" t="s">
         <v>323</v>
       </c>
-      <c r="K2" s="32" t="s">
+      <c r="K2" s="29" t="s">
         <v>323</v>
       </c>
-      <c r="L2" s="32" t="s">
+      <c r="L2" s="29" t="s">
         <v>323</v>
       </c>
-      <c r="M2" s="32" t="s">
+      <c r="M2" s="29" t="s">
         <v>323</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="O2" s="33" t="s">
+      <c r="O2" s="30" t="s">
         <v>324</v>
       </c>
     </row>
@@ -5874,25 +5833,24 @@
       <c r="B1" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="31" t="s">
         <v>326</v>
       </c>
-      <c r="E1" s="35">
-        <f>SUM(B2:B157)</f>
+      <c r="E1" s="32">
+        <v>15072</v>
+      </c>
+      <c r="F1" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="34" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2" s="35">
         <v>18</v>
       </c>
-      <c r="F1" s="36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
-        <v>294</v>
-      </c>
-      <c r="B2" s="38">
-        <v>18</v>
-      </c>
-      <c r="C2" s="36">
+      <c r="C2" s="33">
         <v>1.190318740907287E-3</v>
       </c>
     </row>

</xml_diff>